<commit_message>
fixed some naming errors
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v07_kh_06-10-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v07_kh_06-10-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E188AC07-7FD5-4CD5-A656-E23481E01BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD10DB77-BD1A-419C-8A1D-F317E1FD7585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -509,9 +509,6 @@
     <t>RES_PV_Utility_Opt</t>
   </si>
   <si>
-    <t>Res_PV_Utility_Tracking</t>
-  </si>
-  <si>
     <t>RES_Residues</t>
   </si>
   <si>
@@ -894,6 +891,9 @@
   </si>
   <si>
     <t>X_SOEC_Electrolysis</t>
+  </si>
+  <si>
+    <t>RES_PV_Utility_Tracking</t>
   </si>
 </sst>
 </file>
@@ -945,7 +945,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -961,7 +961,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1259,18 +1259,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1719,21 +1719,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B144"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>153</v>
+        <v>281</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2930,19 +2930,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2974,7 +2974,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3017,19 +3017,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3093,7 +3093,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3288,14 +3288,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,19 +3343,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3374,19 +3374,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3474,7 +3474,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3522,7 +3522,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3541,19 +3541,19 @@
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3624,15 +3624,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>
@@ -3644,7 +3644,7 @@
         <v>2015</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>2019</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3668,7 +3668,7 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>